<commit_message>
phat hanh hoa don dong loat
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/HoaDonDienTu/PHAT_HANH_HOA_DON_LOI.xlsx
+++ b/API/wwwroot/docs/HoaDonDienTu/PHAT_HANH_HOA_DON_LOI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\HoaDonDienTu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD0AB68-EAA1-4EB3-9D19-6A226FB4C40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B3F213-BD85-45E1-BD35-F9DEE7117F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>STT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Ngày hóa đơn</t>
   </si>
@@ -44,38 +41,23 @@
     <t>Số hóa đơn</t>
   </si>
   <si>
-    <t>Ký hiệu mẫu số hóa đơn</t>
-  </si>
-  <si>
-    <t>Ký hiệu hóa đơn</t>
-  </si>
-  <si>
-    <t>Mã khách hàng</t>
-  </si>
-  <si>
     <t>Tên khách hàng</t>
   </si>
   <si>
-    <t>Mã số thuế</t>
+    <t>Ký hiệu</t>
   </si>
   <si>
-    <t>Người mua hàng</t>
+    <t>Trạng thái quy trình</t>
   </si>
   <si>
-    <t>Loại tiền</t>
-  </si>
-  <si>
-    <t>Tổng tiền thanh toán</t>
-  </si>
-  <si>
-    <t>Tình trạng</t>
+    <t>Mô tả lỗi và hướng dẫn cách khắc phục</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,12 +89,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -171,16 +147,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -498,39 +471,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="1" max="1" width="14.875" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="14.875" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="8" width="19.25" customWidth="1"/>
-    <col min="9" max="9" width="31.875" customWidth="1"/>
-    <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="21.125" customWidth="1"/>
-    <col min="12" max="12" width="34" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="34.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -538,38 +506,14 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>